<commit_message>
Misc changes of DFT data and gitignore
</commit_message>
<xml_diff>
--- a/other/DFTOutputComparer.xlsx
+++ b/other/DFTOutputComparer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caibi\Development\CCHW\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25299317-FB5A-429D-96A1-84B3F1E5637F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F29487-63FC-44C0-A5F2-A76F7A41B7F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B47C612-C474-4B91-BE2C-CA782D74DD8D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B47C612-C474-4B91-BE2C-CA782D74DD8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -127,7 +127,7 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -226,10 +226,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.8017545960266916E-2"/>
-          <c:y val="6.5276512372459516E-2"/>
-          <c:w val="0.94374193450293731"/>
-          <c:h val="0.84941257961657435"/>
+          <c:x val="8.3271227460203837E-2"/>
+          <c:y val="8.7568499282095924E-2"/>
+          <c:w val="0.90933933258342692"/>
+          <c:h val="0.80482882639359399"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1801,7 +1801,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-CA"/>
-                  <a:t>Frequency</a:t>
+                  <a:t>Frequency (Hz)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2044,9 +2044,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.9447167417902178E-2"/>
-          <c:y val="6.7059648182659845E-2"/>
-          <c:w val="6.9953330693201157E-2"/>
+          <c:x val="9.1005624296962878E-2"/>
+          <c:y val="7.2632715713498358E-2"/>
+          <c:w val="0.1045853359239186"/>
           <c:h val="7.8878721858044884E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3858,15 +3858,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>100013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3894,15 +3894,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4231,7 +4231,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
+      <selection pane="bottomLeft" activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4304,7 +4304,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <f>POWER(2,A3/24)*$D$2</f>
+        <f t="shared" ref="D3:D34" si="0">POWER(2,A3/24)*$D$2</f>
         <v>56.611623015392063</v>
       </c>
       <c r="E3">
@@ -4332,7 +4332,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="1">
-        <f>POWER(2,A4/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>58.270470189761241</v>
       </c>
       <c r="E4">
@@ -4343,11 +4343,11 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4">
-        <f>E2+E26+E50+E74+E98</f>
+        <f t="shared" ref="H4:H27" si="1">E2+E26+E50+E74+E98</f>
         <v>143899008</v>
       </c>
       <c r="I4">
-        <f>F2+F26+F50+F74+F98</f>
+        <f t="shared" ref="I4:I27" si="2">F2+F26+F50+F74+F98</f>
         <v>279153691</v>
       </c>
     </row>
@@ -4362,7 +4362,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <f>POWER(2,A5/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>59.97792529658917</v>
       </c>
       <c r="E5">
@@ -4373,11 +4373,11 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5">
-        <f>E3+E27+E51+E75+E99</f>
+        <f t="shared" si="1"/>
         <v>1727959846</v>
       </c>
       <c r="I5">
-        <f>F3+F27+F51+F75+F99</f>
+        <f t="shared" si="2"/>
         <v>1527160265</v>
       </c>
     </row>
@@ -4392,7 +4392,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <f>POWER(2,A6/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>61.735412657015516</v>
       </c>
       <c r="E6">
@@ -4403,11 +4403,11 @@
       </c>
       <c r="G6" s="2"/>
       <c r="H6">
-        <f>E4+E28+E52+E76+E100</f>
+        <f t="shared" si="1"/>
         <v>242123508</v>
       </c>
       <c r="I6">
-        <f>F4+F28+F52+F76+F100</f>
+        <f t="shared" si="2"/>
         <v>69760683</v>
       </c>
     </row>
@@ -4422,7 +4422,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="1">
-        <f>POWER(2,A7/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>63.54439832797501</v>
       </c>
       <c r="E7">
@@ -4433,11 +4433,11 @@
       </c>
       <c r="G7" s="2"/>
       <c r="H7">
-        <f>E5+E29+E53+E77+E101</f>
+        <f t="shared" si="1"/>
         <v>129227097</v>
       </c>
       <c r="I7">
-        <f>F5+F29+F53+F77+F101</f>
+        <f t="shared" si="2"/>
         <v>162268955</v>
       </c>
     </row>
@@ -4452,7 +4452,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="1">
-        <f>POWER(2,A8/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>65.406391325149656</v>
       </c>
       <c r="E8">
@@ -4463,11 +4463,11 @@
       </c>
       <c r="G8" s="2"/>
       <c r="H8">
-        <f>E6+E30+E54+E78+E102</f>
+        <f t="shared" si="1"/>
         <v>106968139</v>
       </c>
       <c r="I8">
-        <f>F6+F30+F54+F78+F102</f>
+        <f t="shared" si="2"/>
         <v>121103116</v>
       </c>
     </row>
@@ -4482,7 +4482,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="1">
-        <f>POWER(2,A9/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>67.322944881756044</v>
       </c>
       <c r="E9">
@@ -4493,11 +4493,11 @@
       </c>
       <c r="G9" s="2"/>
       <c r="H9">
-        <f>E7+E31+E55+E79+E103</f>
+        <f t="shared" si="1"/>
         <v>141314151</v>
       </c>
       <c r="I9">
-        <f>F7+F31+F55+F79+F103</f>
+        <f t="shared" si="2"/>
         <v>109252902</v>
       </c>
     </row>
@@ -4512,7 +4512,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="1">
-        <f>POWER(2,A10/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>69.295657744218019</v>
       </c>
       <c r="E10">
@@ -4523,11 +4523,11 @@
       </c>
       <c r="G10" s="2"/>
       <c r="H10">
-        <f>E8+E32+E56+E80+E104</f>
+        <f t="shared" si="1"/>
         <v>154332346</v>
       </c>
       <c r="I10">
-        <f>F8+F32+F56+F80+F104</f>
+        <f t="shared" si="2"/>
         <v>135103343</v>
       </c>
     </row>
@@ -4542,7 +4542,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="1">
-        <f>POWER(2,A11/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>71.326175505805537</v>
       </c>
       <c r="E11">
@@ -4553,11 +4553,11 @@
       </c>
       <c r="G11" s="2"/>
       <c r="H11">
-        <f>E9+E33+E57+E81+E105</f>
+        <f t="shared" si="1"/>
         <v>94364231</v>
       </c>
       <c r="I11">
-        <f>F9+F33+F57+F81+F105</f>
+        <f t="shared" si="2"/>
         <v>96675749</v>
       </c>
     </row>
@@ -4572,7 +4572,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="1">
-        <f>POWER(2,A12/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>73.416191979351893</v>
       </c>
       <c r="E12">
@@ -4583,11 +4583,11 @@
       </c>
       <c r="G12" s="2"/>
       <c r="H12">
-        <f>E10+E34+E58+E82+E106</f>
+        <f t="shared" si="1"/>
         <v>78672896</v>
       </c>
       <c r="I12">
-        <f>F10+F34+F58+F82+F106</f>
+        <f t="shared" si="2"/>
         <v>124577967</v>
       </c>
     </row>
@@ -4602,7 +4602,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="1">
-        <f>POWER(2,A13/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>75.567450610194896</v>
       </c>
       <c r="E13">
@@ -4613,11 +4613,11 @@
       </c>
       <c r="G13" s="2"/>
       <c r="H13">
-        <f>E11+E35+E59+E83+E107</f>
+        <f t="shared" si="1"/>
         <v>105484875</v>
       </c>
       <c r="I13">
-        <f>F11+F35+F59+F83+F107</f>
+        <f t="shared" si="2"/>
         <v>108281534</v>
       </c>
     </row>
@@ -4632,7 +4632,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="1">
-        <f>POWER(2,A14/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>77.781745930520231</v>
       </c>
       <c r="E14">
@@ -4643,11 +4643,11 @@
       </c>
       <c r="G14" s="2"/>
       <c r="H14">
-        <f>E12+E36+E60+E84+E108</f>
+        <f t="shared" si="1"/>
         <v>174920364</v>
       </c>
       <c r="I14">
-        <f>F12+F36+F60+F84+F108</f>
+        <f t="shared" si="2"/>
         <v>154680775</v>
       </c>
     </row>
@@ -4662,7 +4662,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="1">
-        <f>POWER(2,A15/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>80.060925056320301</v>
       </c>
       <c r="E15">
@@ -4673,11 +4673,11 @@
       </c>
       <c r="G15" s="2"/>
       <c r="H15">
-        <f>E13+E37+E61+E85+E109</f>
+        <f t="shared" si="1"/>
         <v>212871747</v>
       </c>
       <c r="I15">
-        <f>F13+F37+F61+F85+F109</f>
+        <f t="shared" si="2"/>
         <v>54116681</v>
       </c>
     </row>
@@ -4692,7 +4692,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="1">
-        <f>POWER(2,A16/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>82.40688922821748</v>
       </c>
       <c r="E16">
@@ -4703,11 +4703,11 @@
       </c>
       <c r="G16" s="2"/>
       <c r="H16">
-        <f>E14+E38+E62+E86+E110</f>
+        <f t="shared" si="1"/>
         <v>262019956</v>
       </c>
       <c r="I16">
-        <f>F14+F38+F62+F86+F110</f>
+        <f t="shared" si="2"/>
         <v>228805002</v>
       </c>
     </row>
@@ -4722,7 +4722,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="1">
-        <f>POWER(2,A17/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>84.821595397436738</v>
       </c>
       <c r="E17">
@@ -4733,11 +4733,11 @@
       </c>
       <c r="G17" s="2"/>
       <c r="H17">
-        <f>E15+E39+E63+E87+E111</f>
+        <f t="shared" si="1"/>
         <v>380433102</v>
       </c>
       <c r="I17">
-        <f>F15+F39+F63+F87+F111</f>
+        <f t="shared" si="2"/>
         <v>266341234</v>
       </c>
     </row>
@@ -4752,7 +4752,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="1">
-        <f>POWER(2,A18/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>87.307057858250971</v>
       </c>
       <c r="E18">
@@ -4763,11 +4763,11 @@
       </c>
       <c r="G18" s="2"/>
       <c r="H18">
-        <f>E16+E40+E64+E88+E112</f>
+        <f t="shared" si="1"/>
         <v>913908432</v>
       </c>
       <c r="I18">
-        <f>F16+F40+F64+F88+F112</f>
+        <f t="shared" si="2"/>
         <v>162317395</v>
       </c>
     </row>
@@ -4782,7 +4782,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="1">
-        <f>POWER(2,A19/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>89.865349928260486</v>
       </c>
       <c r="E19">
@@ -4793,11 +4793,11 @@
       </c>
       <c r="G19" s="2"/>
       <c r="H19">
-        <f>E17+E41+E65+E89+E113</f>
+        <f t="shared" si="1"/>
         <v>1159769925</v>
       </c>
       <c r="I19">
-        <f>F17+F41+F65+F89+F113</f>
+        <f t="shared" si="2"/>
         <v>1419096494</v>
       </c>
     </row>
@@ -4812,7 +4812,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="1">
-        <f>POWER(2,A20/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>92.4986056779086</v>
       </c>
       <c r="E20">
@@ -4823,11 +4823,11 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20">
-        <f>E18+E42+E66+E90+E114</f>
+        <f t="shared" si="1"/>
         <v>381360102</v>
       </c>
       <c r="I20">
-        <f>F18+F42+F66+F90+F114</f>
+        <f t="shared" si="2"/>
         <v>629211629</v>
       </c>
     </row>
@@ -4842,7 +4842,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="1">
-        <f>POWER(2,A21/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>95.209021710675728</v>
       </c>
       <c r="E21">
@@ -4853,11 +4853,11 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21">
-        <f>E19+E43+E67+E91+E115</f>
+        <f t="shared" si="1"/>
         <v>246097229</v>
       </c>
       <c r="I21">
-        <f>F19+F43+F67+F91+F115</f>
+        <f t="shared" si="2"/>
         <v>366625021</v>
       </c>
     </row>
@@ -4872,7 +4872,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="1">
-        <f>POWER(2,A22/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>97.998858995437317</v>
       </c>
       <c r="E22">
@@ -4883,11 +4883,11 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22">
-        <f>E20+E44+E68+E92+E116</f>
+        <f t="shared" si="1"/>
         <v>216107104</v>
       </c>
       <c r="I22">
-        <f>F20+F44+F68+F92+F116</f>
+        <f t="shared" si="2"/>
         <v>246470151</v>
       </c>
     </row>
@@ -4902,7 +4902,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="1">
-        <f>POWER(2,A23/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>100.87044475251383</v>
       </c>
       <c r="E23">
@@ -4913,11 +4913,11 @@
       </c>
       <c r="G23" s="2"/>
       <c r="H23">
-        <f>E21+E45+E69+E93+E117</f>
+        <f t="shared" si="1"/>
         <v>132620919</v>
       </c>
       <c r="I23">
-        <f>F21+F45+F69+F93+F117</f>
+        <f t="shared" si="2"/>
         <v>197818736</v>
       </c>
     </row>
@@ -4932,7 +4932,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="1">
-        <f>POWER(2,A24/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>103.82617439498628</v>
       </c>
       <c r="E24">
@@ -4943,11 +4943,11 @@
       </c>
       <c r="G24" s="2"/>
       <c r="H24">
-        <f>E22+E46+E70+E94+E118</f>
+        <f t="shared" si="1"/>
         <v>85077402</v>
       </c>
       <c r="I24">
-        <f>F22+F46+F70+F94+F118</f>
+        <f t="shared" si="2"/>
         <v>185517540</v>
       </c>
     </row>
@@ -4962,7 +4962,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="1">
-        <f>POWER(2,A25/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>106.86851352689665</v>
       </c>
       <c r="E25">
@@ -4973,11 +4973,11 @@
       </c>
       <c r="G25" s="2"/>
       <c r="H25">
-        <f>E23+E47+E71+E95+E119</f>
+        <f t="shared" si="1"/>
         <v>199044320</v>
       </c>
       <c r="I25">
-        <f>F23+F47+F71+F95+F119</f>
+        <f t="shared" si="2"/>
         <v>233358029</v>
       </c>
     </row>
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="1">
-        <f>POWER(2,A26/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>110</v>
       </c>
       <c r="E26">
@@ -5003,11 +5003,11 @@
       </c>
       <c r="G26" s="2"/>
       <c r="H26">
-        <f>E24+E48+E72+E96+E120</f>
+        <f t="shared" si="1"/>
         <v>285364491</v>
       </c>
       <c r="I26">
-        <f>F24+F48+F72+F96+F120</f>
+        <f t="shared" si="2"/>
         <v>300143718</v>
       </c>
     </row>
@@ -5022,7 +5022,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="1">
-        <f>POWER(2,A27/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>113.22324603078413</v>
       </c>
       <c r="E27">
@@ -5033,11 +5033,11 @@
       </c>
       <c r="G27" s="2"/>
       <c r="H27">
-        <f>E25+E49+E73+E97+E121</f>
+        <f t="shared" si="1"/>
         <v>473343831</v>
       </c>
       <c r="I27">
-        <f>F25+F49+F73+F97+F121</f>
+        <f t="shared" si="2"/>
         <v>298052929</v>
       </c>
     </row>
@@ -5052,7 +5052,7 @@
         <v>2</v>
       </c>
       <c r="D28" s="1">
-        <f>POWER(2,A28/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>116.54094037952245</v>
       </c>
       <c r="E28">
@@ -5074,7 +5074,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="1">
-        <f>POWER(2,A29/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>119.95585059317834</v>
       </c>
       <c r="E29">
@@ -5096,7 +5096,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="1">
-        <f>POWER(2,A30/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>123.47082531403103</v>
       </c>
       <c r="E30">
@@ -5118,7 +5118,7 @@
         <v>5</v>
       </c>
       <c r="D31" s="1">
-        <f>POWER(2,A31/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>127.08879665595002</v>
       </c>
       <c r="E31">
@@ -5140,7 +5140,7 @@
         <v>6</v>
       </c>
       <c r="D32" s="1">
-        <f>POWER(2,A32/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>130.81278265029931</v>
       </c>
       <c r="E32">
@@ -5162,7 +5162,7 @@
         <v>7</v>
       </c>
       <c r="D33" s="1">
-        <f>POWER(2,A33/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>134.64588976351209</v>
       </c>
       <c r="E33">
@@ -5184,7 +5184,7 @@
         <v>8</v>
       </c>
       <c r="D34" s="1">
-        <f>POWER(2,A34/24)*$D$2</f>
+        <f t="shared" si="0"/>
         <v>138.59131548843604</v>
       </c>
       <c r="E34">
@@ -5206,7 +5206,7 @@
         <v>9</v>
       </c>
       <c r="D35" s="1">
-        <f>POWER(2,A35/24)*$D$2</f>
+        <f t="shared" ref="D35:D66" si="3">POWER(2,A35/24)*$D$2</f>
         <v>142.65235101161107</v>
       </c>
       <c r="E35">
@@ -5228,7 +5228,7 @@
         <v>10</v>
       </c>
       <c r="D36" s="1">
-        <f>POWER(2,A36/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>146.83238395870379</v>
       </c>
       <c r="E36">
@@ -5250,7 +5250,7 @@
         <v>11</v>
       </c>
       <c r="D37" s="1">
-        <f>POWER(2,A37/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>151.13490122038979</v>
       </c>
       <c r="E37">
@@ -5272,7 +5272,7 @@
         <v>12</v>
       </c>
       <c r="D38" s="1">
-        <f>POWER(2,A38/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>155.56349186104043</v>
       </c>
       <c r="E38">
@@ -5294,7 +5294,7 @@
         <v>13</v>
       </c>
       <c r="D39" s="1">
-        <f>POWER(2,A39/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>160.1218501126406</v>
       </c>
       <c r="E39">
@@ -5317,7 +5317,7 @@
         <v>14</v>
       </c>
       <c r="D40" s="1">
-        <f>POWER(2,A40/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>164.81377845643493</v>
       </c>
       <c r="E40">
@@ -5339,7 +5339,7 @@
         <v>15</v>
       </c>
       <c r="D41" s="1">
-        <f>POWER(2,A41/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>169.64319079487348</v>
       </c>
       <c r="E41">
@@ -5362,7 +5362,7 @@
         <v>16</v>
       </c>
       <c r="D42" s="1">
-        <f>POWER(2,A42/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>174.61411571650194</v>
       </c>
       <c r="E42">
@@ -5385,7 +5385,7 @@
         <v>17</v>
       </c>
       <c r="D43" s="1">
-        <f>POWER(2,A43/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>179.73069985652094</v>
       </c>
       <c r="E43">
@@ -5408,7 +5408,7 @@
         <v>18</v>
       </c>
       <c r="D44" s="1">
-        <f>POWER(2,A44/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>184.9972113558172</v>
       </c>
       <c r="E44">
@@ -5431,7 +5431,7 @@
         <v>19</v>
       </c>
       <c r="D45" s="1">
-        <f>POWER(2,A45/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>190.41804342135148</v>
       </c>
       <c r="E45">
@@ -5453,7 +5453,7 @@
         <v>20</v>
       </c>
       <c r="D46" s="1">
-        <f>POWER(2,A46/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>195.99771799087461</v>
       </c>
       <c r="E46">
@@ -5475,7 +5475,7 @@
         <v>21</v>
       </c>
       <c r="D47" s="1">
-        <f>POWER(2,A47/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>201.74088950502767</v>
       </c>
       <c r="E47">
@@ -5497,7 +5497,7 @@
         <v>22</v>
       </c>
       <c r="D48" s="1">
-        <f>POWER(2,A48/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>207.65234878997256</v>
       </c>
       <c r="E48">
@@ -5519,7 +5519,7 @@
         <v>23</v>
       </c>
       <c r="D49" s="1">
-        <f>POWER(2,A49/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>213.73702705379327</v>
       </c>
       <c r="E49">
@@ -5541,7 +5541,7 @@
         <v>0</v>
       </c>
       <c r="D50" s="1">
-        <f>POWER(2,A50/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>220</v>
       </c>
       <c r="E50">
@@ -5563,7 +5563,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="1">
-        <f>POWER(2,A51/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>226.44649206156822</v>
       </c>
       <c r="E51">
@@ -5585,7 +5585,7 @@
         <v>2</v>
       </c>
       <c r="D52" s="1">
-        <f>POWER(2,A52/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>233.08188075904496</v>
       </c>
       <c r="E52">
@@ -5607,7 +5607,7 @@
         <v>3</v>
       </c>
       <c r="D53" s="1">
-        <f>POWER(2,A53/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>239.91170118635668</v>
       </c>
       <c r="E53">
@@ -5629,7 +5629,7 @@
         <v>4</v>
       </c>
       <c r="D54" s="1">
-        <f>POWER(2,A54/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>246.94165062806201</v>
       </c>
       <c r="E54">
@@ -5651,7 +5651,7 @@
         <v>5</v>
       </c>
       <c r="D55" s="1">
-        <f>POWER(2,A55/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>254.1775933119001</v>
       </c>
       <c r="E55">
@@ -5673,7 +5673,7 @@
         <v>6</v>
       </c>
       <c r="D56" s="1">
-        <f>POWER(2,A56/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>261.62556530059862</v>
       </c>
       <c r="E56">
@@ -5695,7 +5695,7 @@
         <v>7</v>
       </c>
       <c r="D57" s="1">
-        <f>POWER(2,A57/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>269.29177952702412</v>
       </c>
       <c r="E57">
@@ -5717,7 +5717,7 @@
         <v>8</v>
       </c>
       <c r="D58" s="1">
-        <f>POWER(2,A58/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>277.18263097687213</v>
       </c>
       <c r="E58">
@@ -5739,7 +5739,7 @@
         <v>9</v>
       </c>
       <c r="D59" s="1">
-        <f>POWER(2,A59/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>285.30470202322215</v>
       </c>
       <c r="E59">
@@ -5761,7 +5761,7 @@
         <v>10</v>
       </c>
       <c r="D60" s="1">
-        <f>POWER(2,A60/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>293.66476791740752</v>
       </c>
       <c r="E60">
@@ -5783,7 +5783,7 @@
         <v>11</v>
       </c>
       <c r="D61" s="1">
-        <f>POWER(2,A61/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>302.26980244077964</v>
       </c>
       <c r="E61">
@@ -5805,7 +5805,7 @@
         <v>12</v>
       </c>
       <c r="D62" s="1">
-        <f>POWER(2,A62/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>311.12698372208092</v>
       </c>
       <c r="E62">
@@ -5827,7 +5827,7 @@
         <v>13</v>
       </c>
       <c r="D63" s="1">
-        <f>POWER(2,A63/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>320.24370022528115</v>
       </c>
       <c r="E63">
@@ -5849,7 +5849,7 @@
         <v>14</v>
       </c>
       <c r="D64" s="1">
-        <f>POWER(2,A64/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>329.62755691286998</v>
       </c>
       <c r="E64">
@@ -5871,7 +5871,7 @@
         <v>15</v>
       </c>
       <c r="D65" s="1">
-        <f>POWER(2,A65/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>339.28638158974695</v>
       </c>
       <c r="E65">
@@ -5893,7 +5893,7 @@
         <v>16</v>
       </c>
       <c r="D66" s="1">
-        <f>POWER(2,A66/24)*$D$2</f>
+        <f t="shared" si="3"/>
         <v>349.22823143300388</v>
       </c>
       <c r="E66">
@@ -5915,7 +5915,7 @@
         <v>17</v>
       </c>
       <c r="D67" s="1">
-        <f>POWER(2,A67/24)*$D$2</f>
+        <f t="shared" ref="D67:D98" si="4">POWER(2,A67/24)*$D$2</f>
         <v>359.46139971304194</v>
       </c>
       <c r="E67">
@@ -5937,7 +5937,7 @@
         <v>18</v>
       </c>
       <c r="D68" s="1">
-        <f>POWER(2,A68/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>369.99442271163446</v>
       </c>
       <c r="E68">
@@ -5959,7 +5959,7 @@
         <v>19</v>
       </c>
       <c r="D69" s="1">
-        <f>POWER(2,A69/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>380.83608684270291</v>
       </c>
       <c r="E69">
@@ -5981,7 +5981,7 @@
         <v>20</v>
       </c>
       <c r="D70" s="1">
-        <f>POWER(2,A70/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>391.99543598174927</v>
       </c>
       <c r="E70">
@@ -6003,7 +6003,7 @@
         <v>21</v>
       </c>
       <c r="D71" s="1">
-        <f>POWER(2,A71/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>403.48177901005533</v>
       </c>
       <c r="E71">
@@ -6026,7 +6026,7 @@
         <v>22</v>
       </c>
       <c r="D72" s="1">
-        <f>POWER(2,A72/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>415.30469757994501</v>
       </c>
       <c r="E72">
@@ -6048,7 +6048,7 @@
         <v>23</v>
       </c>
       <c r="D73" s="1">
-        <f>POWER(2,A73/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>427.47405410758665</v>
       </c>
       <c r="E73">
@@ -6071,7 +6071,7 @@
         <v>0</v>
       </c>
       <c r="D74" s="1">
-        <f>POWER(2,A74/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>440</v>
       </c>
       <c r="E74">
@@ -6094,7 +6094,7 @@
         <v>1</v>
       </c>
       <c r="D75" s="1">
-        <f>POWER(2,A75/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>452.89298412313644</v>
       </c>
       <c r="E75">
@@ -6117,7 +6117,7 @@
         <v>2</v>
       </c>
       <c r="D76" s="1">
-        <f>POWER(2,A76/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>466.16376151808993</v>
       </c>
       <c r="E76">
@@ -6140,7 +6140,7 @@
         <v>3</v>
       </c>
       <c r="D77" s="1">
-        <f>POWER(2,A77/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>479.82340237271336</v>
       </c>
       <c r="E77">
@@ -6162,7 +6162,7 @@
         <v>4</v>
       </c>
       <c r="D78" s="1">
-        <f>POWER(2,A78/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>493.88330125612396</v>
       </c>
       <c r="E78">
@@ -6184,7 +6184,7 @@
         <v>5</v>
       </c>
       <c r="D79" s="1">
-        <f>POWER(2,A79/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>508.35518662380019</v>
       </c>
       <c r="E79">
@@ -6206,7 +6206,7 @@
         <v>6</v>
       </c>
       <c r="D80" s="1">
-        <f>POWER(2,A80/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>523.25113060119713</v>
       </c>
       <c r="E80">
@@ -6228,7 +6228,7 @@
         <v>7</v>
       </c>
       <c r="D81" s="1">
-        <f>POWER(2,A81/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>538.58355905404824</v>
       </c>
       <c r="E81">
@@ -6250,7 +6250,7 @@
         <v>8</v>
       </c>
       <c r="D82" s="1">
-        <f>POWER(2,A82/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>554.36526195374415</v>
       </c>
       <c r="E82">
@@ -6272,7 +6272,7 @@
         <v>9</v>
       </c>
       <c r="D83" s="1">
-        <f>POWER(2,A83/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>570.6094040464443</v>
       </c>
       <c r="E83">
@@ -6294,7 +6294,7 @@
         <v>10</v>
       </c>
       <c r="D84" s="1">
-        <f>POWER(2,A84/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>587.32953583481492</v>
       </c>
       <c r="E84">
@@ -6316,7 +6316,7 @@
         <v>11</v>
       </c>
       <c r="D85" s="1">
-        <f>POWER(2,A85/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>604.53960488155928</v>
       </c>
       <c r="E85">
@@ -6338,7 +6338,7 @@
         <v>12</v>
       </c>
       <c r="D86" s="1">
-        <f>POWER(2,A86/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>622.25396744416173</v>
       </c>
       <c r="E86">
@@ -6360,7 +6360,7 @@
         <v>13</v>
       </c>
       <c r="D87" s="1">
-        <f>POWER(2,A87/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>640.4874004505624</v>
       </c>
       <c r="E87">
@@ -6382,7 +6382,7 @@
         <v>14</v>
       </c>
       <c r="D88" s="1">
-        <f>POWER(2,A88/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>659.25511382573984</v>
       </c>
       <c r="E88">
@@ -6404,7 +6404,7 @@
         <v>15</v>
       </c>
       <c r="D89" s="1">
-        <f>POWER(2,A89/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>678.57276317949402</v>
       </c>
       <c r="E89">
@@ -6426,7 +6426,7 @@
         <v>16</v>
       </c>
       <c r="D90" s="1">
-        <f>POWER(2,A90/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>698.45646286600766</v>
       </c>
       <c r="E90">
@@ -6448,7 +6448,7 @@
         <v>17</v>
       </c>
       <c r="D91" s="1">
-        <f>POWER(2,A91/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>718.92279942608377</v>
       </c>
       <c r="E91">
@@ -6470,7 +6470,7 @@
         <v>18</v>
       </c>
       <c r="D92" s="1">
-        <f>POWER(2,A92/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>739.9888454232688</v>
       </c>
       <c r="E92">
@@ -6492,7 +6492,7 @@
         <v>19</v>
       </c>
       <c r="D93" s="1">
-        <f>POWER(2,A93/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>761.67217368540582</v>
       </c>
       <c r="E93">
@@ -6514,7 +6514,7 @@
         <v>20</v>
       </c>
       <c r="D94" s="1">
-        <f>POWER(2,A94/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>783.99087196349865</v>
       </c>
       <c r="E94">
@@ -6536,7 +6536,7 @@
         <v>21</v>
       </c>
       <c r="D95" s="1">
-        <f>POWER(2,A95/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>806.96355802011078</v>
       </c>
       <c r="E95">
@@ -6558,7 +6558,7 @@
         <v>22</v>
       </c>
       <c r="D96" s="1">
-        <f>POWER(2,A96/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>830.60939515989014</v>
       </c>
       <c r="E96">
@@ -6580,7 +6580,7 @@
         <v>23</v>
       </c>
       <c r="D97" s="1">
-        <f>POWER(2,A97/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>854.94810821517308</v>
       </c>
       <c r="E97">
@@ -6602,7 +6602,7 @@
         <v>0</v>
       </c>
       <c r="D98" s="1">
-        <f>POWER(2,A98/24)*$D$2</f>
+        <f t="shared" si="4"/>
         <v>880</v>
       </c>
       <c r="E98">
@@ -6625,7 +6625,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="1">
-        <f>POWER(2,A99/24)*$D$2</f>
+        <f t="shared" ref="D99:D121" si="5">POWER(2,A99/24)*$D$2</f>
         <v>905.785968246273</v>
       </c>
       <c r="E99">
@@ -6647,7 +6647,7 @@
         <v>2</v>
       </c>
       <c r="D100" s="1">
-        <f>POWER(2,A100/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>932.32752303617951</v>
       </c>
       <c r="E100">
@@ -6670,7 +6670,7 @@
         <v>3</v>
       </c>
       <c r="D101" s="1">
-        <f>POWER(2,A101/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>959.64680474542638</v>
       </c>
       <c r="E101">
@@ -6693,7 +6693,7 @@
         <v>4</v>
       </c>
       <c r="D102" s="1">
-        <f>POWER(2,A102/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>987.76660251224848</v>
       </c>
       <c r="E102">
@@ -6716,7 +6716,7 @@
         <v>5</v>
       </c>
       <c r="D103" s="1">
-        <f>POWER(2,A103/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1016.7103732476002</v>
       </c>
       <c r="E103">
@@ -6739,7 +6739,7 @@
         <v>6</v>
       </c>
       <c r="D104" s="1">
-        <f>POWER(2,A104/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1046.5022612023945</v>
       </c>
       <c r="E104">
@@ -6761,7 +6761,7 @@
         <v>7</v>
       </c>
       <c r="D105" s="1">
-        <f>POWER(2,A105/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1077.1671181080967</v>
       </c>
       <c r="E105">
@@ -6783,7 +6783,7 @@
         <v>8</v>
       </c>
       <c r="D106" s="1">
-        <f>POWER(2,A106/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1108.7305239074881</v>
       </c>
       <c r="E106">
@@ -6805,7 +6805,7 @@
         <v>9</v>
       </c>
       <c r="D107" s="1">
-        <f>POWER(2,A107/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1141.2188080928881</v>
       </c>
       <c r="E107">
@@ -6827,7 +6827,7 @@
         <v>10</v>
       </c>
       <c r="D108" s="1">
-        <f>POWER(2,A108/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1174.6590716696305</v>
       </c>
       <c r="E108">
@@ -6849,7 +6849,7 @@
         <v>11</v>
       </c>
       <c r="D109" s="1">
-        <f>POWER(2,A109/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1209.0792097631183</v>
       </c>
       <c r="E109">
@@ -6871,7 +6871,7 @@
         <v>12</v>
       </c>
       <c r="D110" s="1">
-        <f>POWER(2,A110/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1244.5079348883235</v>
       </c>
       <c r="E110">
@@ -6893,7 +6893,7 @@
         <v>13</v>
       </c>
       <c r="D111" s="1">
-        <f>POWER(2,A111/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1280.974800901125</v>
       </c>
       <c r="E111">
@@ -6915,7 +6915,7 @@
         <v>14</v>
       </c>
       <c r="D112" s="1">
-        <f>POWER(2,A112/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1318.5102276514795</v>
       </c>
       <c r="E112">
@@ -6937,7 +6937,7 @@
         <v>15</v>
       </c>
       <c r="D113" s="1">
-        <f>POWER(2,A113/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1357.1455263589876</v>
       </c>
       <c r="E113">
@@ -6959,7 +6959,7 @@
         <v>16</v>
       </c>
       <c r="D114" s="1">
-        <f>POWER(2,A114/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1396.9129257320158</v>
       </c>
       <c r="E114">
@@ -6981,7 +6981,7 @@
         <v>17</v>
       </c>
       <c r="D115" s="1">
-        <f>POWER(2,A115/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1437.8455988521678</v>
       </c>
       <c r="E115">
@@ -7003,7 +7003,7 @@
         <v>18</v>
       </c>
       <c r="D116" s="1">
-        <f>POWER(2,A116/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1479.9776908465376</v>
       </c>
       <c r="E116">
@@ -7025,7 +7025,7 @@
         <v>19</v>
       </c>
       <c r="D117" s="1">
-        <f>POWER(2,A117/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1523.3443473708119</v>
       </c>
       <c r="E117">
@@ -7047,7 +7047,7 @@
         <v>20</v>
       </c>
       <c r="D118" s="1">
-        <f>POWER(2,A118/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1567.9817439269968</v>
       </c>
       <c r="E118">
@@ -7069,7 +7069,7 @@
         <v>21</v>
       </c>
       <c r="D119" s="1">
-        <f>POWER(2,A119/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1613.9271160402209</v>
       </c>
       <c r="E119">
@@ -7091,7 +7091,7 @@
         <v>22</v>
       </c>
       <c r="D120" s="1">
-        <f>POWER(2,A120/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1661.218790319781</v>
       </c>
       <c r="E120">
@@ -7113,7 +7113,7 @@
         <v>23</v>
       </c>
       <c r="D121" s="1">
-        <f>POWER(2,A121/24)*$D$2</f>
+        <f t="shared" si="5"/>
         <v>1709.8962164303452</v>
       </c>
       <c r="E121">

</xml_diff>